<commit_message>
EPBDS: added conditionABId to key, updated xls for Class level configuration
</commit_message>
<xml_diff>
--- a/MAPPING/branches/20110624_condition_to_key/org.openl.rules.mapping.dev.test/src/test/resources/org/openl/rules/mapping/config/ClassMappingConfigurationTest.xlsx
+++ b/MAPPING/branches/20110624_condition_to_key/org.openl.rules.mapping.dev.test/src/test/resources/org/openl/rules/mapping/config/ClassMappingConfigurationTest.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="24735" windowHeight="11955"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="19320" windowHeight="11955"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="5" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
   <si>
     <t>classA</t>
   </si>
@@ -119,13 +119,25 @@
   </si>
   <si>
     <t>Data ClassMappingConfiguration classConfiguration</t>
+  </si>
+  <si>
+    <t>classABeanFactory</t>
+  </si>
+  <si>
+    <t>classBBeanFactory</t>
+  </si>
+  <si>
+    <t>Class A Bean Factory</t>
+  </si>
+  <si>
+    <t>Class B Bean Factory</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,6 +257,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -323,6 +340,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -357,6 +375,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -532,32 +551,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C4:J24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C4:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
     <col min="6" max="6" width="23.140625" customWidth="1"/>
     <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.140625" customWidth="1"/>
     <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" customWidth="1"/>
+    <col min="12" max="12" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:9">
+    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="3:9">
+    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C5" s="5" t="s">
         <v>6</v>
       </c>
@@ -565,25 +586,25 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="3:9">
+    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C6" s="5"/>
       <c r="D6" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="3:9">
+    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C7" s="5"/>
       <c r="D7" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="3:9">
+    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C8" s="5"/>
       <c r="D8" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="3:9">
+    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C12" s="6" t="s">
         <v>4</v>
       </c>
@@ -594,7 +615,7 @@
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
     </row>
-    <row r="13" spans="3:9">
+    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C13" s="2" t="s">
         <v>0</v>
       </c>
@@ -617,7 +638,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="3:9">
+    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C14" s="3" t="s">
         <v>8</v>
       </c>
@@ -640,7 +661,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="3:9">
+    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>12</v>
       </c>
@@ -657,7 +678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="3:9">
+    <row r="16" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>12</v>
       </c>
@@ -680,7 +701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="3:10">
+    <row r="21" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C21" s="6" t="s">
         <v>34</v>
       </c>
@@ -691,8 +712,10 @@
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
-    </row>
-    <row r="22" spans="3:10">
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C22" s="2" t="s">
         <v>0</v>
       </c>
@@ -717,8 +740,14 @@
       <c r="J22" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="3:10">
+      <c r="K22" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C23" s="3" t="s">
         <v>8</v>
       </c>
@@ -743,8 +772,14 @@
       <c r="J23" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="24" spans="3:10" ht="15.75">
+      <c r="K23" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="3:12" ht="15.75" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
         <v>12</v>
       </c>
@@ -767,6 +802,32 @@
         <v>25</v>
       </c>
       <c r="J24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="3:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" t="b">
+        <v>0</v>
+      </c>
+      <c r="F25" t="b">
+        <v>1</v>
+      </c>
+      <c r="G25" t="b">
+        <v>0</v>
+      </c>
+      <c r="H25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J25" t="b">
         <v>0</v>
       </c>
     </row>
@@ -774,8 +835,8 @@
   <mergeCells count="4">
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:C8"/>
-    <mergeCell ref="C21:J21"/>
     <mergeCell ref="C12:I12"/>
+    <mergeCell ref="C21:L21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>